<commit_message>
[Document, Modified] : ManagementTask Thiết kế xử lý
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/Thiết Kế Phần Mềm/Thiết Kế Xử Lý/ManagementTask/ManagementTask.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/Thiết Kế Phần Mềm/Thiết Kế Xử Lý/ManagementTask/ManagementTask.xlsx
@@ -7,14 +7,14 @@
     <workbookView windowWidth="19815" windowHeight="7830"/>
   </bookViews>
   <sheets>
-    <sheet name="ManagementTask" sheetId="1" r:id="rId1"/>
+    <sheet name="ManageTask" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="243">
   <si>
     <t>DANH SÁCH CÁC KIỂU DỮ LIỆU XỬ LÝ</t>
   </si>
@@ -80,7 +80,8 @@
   </si>
   <si>
     <t xml:space="preserve"> - Số lượng task
-- Giao diện xem</t>
+- Giao diện xem
+- Trạng thái của task</t>
   </si>
   <si>
     <t>taskId</t>
@@ -89,10 +90,10 @@
     <t>String</t>
   </si>
   <si>
-    <t>TK00001</t>
+    <t>Phải là duy nhất</t>
   </si>
   <si>
-    <t>Phải là duy nhất</t>
+    <t>null</t>
   </si>
   <si>
     <t>Lưu mã task</t>
@@ -119,7 +120,7 @@
     <t>Vét cạn</t>
   </si>
   <si>
-    <t>Đọc danh sách task từ CSDL</t>
+    <t>Truyền sectionId xuống controller và nhận danh sách task  từ controller</t>
   </si>
   <si>
     <t>string</t>
@@ -145,9 +146,6 @@
 của Class Section</t>
   </si>
   <si>
-    <t>SS00001</t>
-  </si>
-  <si>
     <t>Lưu mã section</t>
   </si>
   <si>
@@ -163,22 +161,16 @@
     <t>saveTask bao gồm cả việc thêm và sửa task</t>
   </si>
   <si>
-    <t>addTask()</t>
+    <t>getListTask()</t>
   </si>
   <si>
-    <t>String taskName</t>
-  </si>
-  <si>
-    <t>Thêm task mới</t>
+    <t>Truyền sectionId từ view xuống CSDL và nhận danh sách task từ CSDL</t>
   </si>
   <si>
     <t>double</t>
   </si>
   <si>
     <t>taskName</t>
-  </si>
-  <si>
-    <t>null</t>
   </si>
   <si>
     <t>Không được trùng với 
@@ -197,13 +189,10 @@
     <t>Định nghĩa hành động xóa task</t>
   </si>
   <si>
-    <t>updateTask()</t>
+    <t>selectTask()</t>
   </si>
   <si>
-    <t xml:space="preserve">String taskName, String taskNote, String priorityId, String tagId, String progressId, String repeaterId,Date taskBeginDate, Date taskEndDate, boolean taskFavoriteStatus </t>
-  </si>
-  <si>
-    <t>Sửa task đã có sẵn</t>
+    <t>Truy vấn CSDL để lấy danh sách task của section đó và truyền danh sách task lên controller</t>
   </si>
   <si>
     <t>List</t>
@@ -227,13 +216,10 @@
     <t>Định nghĩa hành động đóng mở form luân phiên</t>
   </si>
   <si>
-    <t>deleteTask()</t>
+    <t>displayTask()</t>
   </si>
   <si>
-    <t>String taskId</t>
-  </si>
-  <si>
-    <t>Xóa task đã có</t>
+    <t>Hiển thị danh sách task lên màn hình</t>
   </si>
   <si>
     <t>boolean</t>
@@ -257,13 +243,13 @@
     <t>Định nghỉ hành động mở form</t>
   </si>
   <si>
-    <t>searchTask()</t>
+    <t>addTask()</t>
   </si>
   <si>
-    <t>String infoSearch</t>
+    <t>String taskName</t>
   </si>
   <si>
-    <t>Tìm kiếm theo tên task</t>
+    <t>Truyền thông tin thêm task xuống controller</t>
   </si>
   <si>
     <t>Set</t>
@@ -295,13 +281,10 @@
     <t xml:space="preserve">Định nghĩa hành động đóng form </t>
   </si>
   <si>
-    <t>sortTask()</t>
+    <t>checkTaskName()</t>
   </si>
   <si>
-    <t>String infoSort</t>
-  </si>
-  <si>
-    <t>Sắp xếp theo tiêu chí</t>
+    <t xml:space="preserve">Kiểm tra tên task sẽ thêm có trùng hay không </t>
   </si>
   <si>
     <t>HashMap</t>
@@ -325,13 +308,7 @@
     <t>Định nghĩa hành động tìm kiếm task</t>
   </si>
   <si>
-    <t>groupByTask()</t>
-  </si>
-  <si>
-    <t>String infoGroupBy</t>
-  </si>
-  <si>
-    <t>Gom nhóm task theo tiêu chí</t>
+    <t>Truyền thông tin thêm task từ controller xuống CSDL</t>
   </si>
   <si>
     <t>Time</t>
@@ -353,13 +330,10 @@
     <t>Số lượng ký tự tối đa của tên task</t>
   </si>
   <si>
-    <t>regexTask()</t>
+    <t>setName()</t>
   </si>
   <si>
-    <t>String infoRegex</t>
-  </si>
-  <si>
-    <t>Tìm kiếm task theo biểu thức chính quy</t>
+    <t>Gán giá trị mới cho tên task</t>
   </si>
   <si>
     <t>Date</t>
@@ -384,13 +358,13 @@
     <t>Số lượng ký tự tối thiểu của tên task</t>
   </si>
   <si>
-    <t>viewTask()</t>
+    <t>getName()</t>
   </si>
   <si>
-    <t>int viewTask</t>
+    <t>String taskId</t>
   </si>
   <si>
-    <t>Chế độ xem dạng List hoặc Board</t>
+    <t xml:space="preserve">Lấy tên task của task </t>
   </si>
   <si>
     <t>infoSort</t>
@@ -399,13 +373,13 @@
     <t>taskBeginDate</t>
   </si>
   <si>
-    <t>Lưu bắt đầu task</t>
+    <t>Lưu ngày bắt đầu task</t>
   </si>
   <si>
-    <t>completeTask()</t>
+    <t>insertTask()</t>
   </si>
   <si>
-    <t>Đánh dấu task hoàn thành</t>
+    <t>Thêm task mới dưới CSDL</t>
   </si>
   <si>
     <t>infoGroupBy</t>
@@ -417,19 +391,43 @@
     <t>Lưu ngày kết thúc task</t>
   </si>
   <si>
+    <t>updateTask()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String taskName, String taskNote, String priorityId, String tagId, String progressId, String repeaterId,Date taskBeginDate, Date taskEndDate, boolean taskFavoriteStatus </t>
+  </si>
+  <si>
+    <t>Truyền thông tin sửa task xuống controller</t>
+  </si>
+  <si>
     <t>infoRegex</t>
   </si>
   <si>
     <t>taskCreateDate</t>
   </si>
   <si>
-    <t>Lưu tạo task</t>
+    <t>Lưu ngày tạo task</t>
+  </si>
+  <si>
+    <t>setTaskNote()</t>
+  </si>
+  <si>
+    <t>String taskNote</t>
+  </si>
+  <si>
+    <t>Gán giá trị mới cho ghi chú của task</t>
   </si>
   <si>
     <t>taskDeleteDate</t>
   </si>
   <si>
-    <t>Lưu xóa task</t>
+    <t>Lưu ngày xóa task</t>
+  </si>
+  <si>
+    <t>getTaskNote()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lấy ghi chú của task </t>
   </si>
   <si>
     <t>DANH SÁCH CÁC THUỘC TÍNH KIỂU DỮ LIỆU int</t>
@@ -444,23 +442,36 @@
     <t>Kết nối xuống lớp DAO</t>
   </si>
   <si>
+    <t>setPriorityId()</t>
+  </si>
+  <si>
+    <t>String priorityId</t>
+  </si>
+  <si>
+    <t>Gán giá trị mới cho mã mức độ ưu tiên của task</t>
+  </si>
+  <si>
     <t>numberOfTask</t>
   </si>
   <si>
     <t>taskFavoriteStatus</t>
   </si>
   <si>
-    <t xml:space="preserve">Lưu task có được yêu thích </t>
+    <t xml:space="preserve">Lưu task có được yêu thích không  </t>
   </si>
   <si>
-    <t>viewTask</t>
+    <t>getPriorityId()</t>
   </si>
   <si>
-    <t xml:space="preserve">int </t>
+    <t xml:space="preserve">Lấy mã mức độ ưu tiên của task </t>
   </si>
   <si>
-    <t>0 : Xem dạng List
-1 : Xem dạng Board</t>
+    <t>taskStatus</t>
+  </si>
+  <si>
+    <t>0: Chưa hoàn thành
+1: Đang làm
+2: Đã hoàn thành</t>
   </si>
   <si>
     <t>taskLate</t>
@@ -469,16 +480,40 @@
     <t>Lưu task có quá hạn không</t>
   </si>
   <si>
-    <t>taskStatusId</t>
+    <t>setTagId()</t>
   </si>
   <si>
-    <t>Lưu task có hoàn thành hay không</t>
+    <t>String tagId</t>
+  </si>
+  <si>
+    <t>Gán giá trị mới cho mã loại của task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lưu trạng thái của task  </t>
+  </si>
+  <si>
+    <t>Có 3 trạng thái: Chưa hoàn thành, Đang làm, Đã hoàn thành</t>
+  </si>
+  <si>
+    <t>getTagId()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lấy mã loại của task </t>
   </si>
   <si>
     <t>DANH SÁCH CÁC THUỘC TÍNH KIỂU DỮ LIỆU TaskDAO</t>
   </si>
   <si>
     <t>Lưu thông tin sắp xếp</t>
+  </si>
+  <si>
+    <t>setProgressId()</t>
+  </si>
+  <si>
+    <t>String progressId</t>
+  </si>
+  <si>
+    <t>Gán giá trị mới cho mã tiến trình của task</t>
   </si>
   <si>
     <t>new TaskDAO()</t>
@@ -491,7 +526,22 @@
     <t>Lưu thông tin gom nhóm</t>
   </si>
   <si>
+    <t>getProgressId()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lấy mã tiến trình của task </t>
+  </si>
+  <si>
     <t>Lưu biểu thức chính quy</t>
+  </si>
+  <si>
+    <t>setRepeaterId()</t>
+  </si>
+  <si>
+    <t>String repeaterId</t>
+  </si>
+  <si>
+    <t>Gán giá trị mới cho mã lặp của task</t>
   </si>
   <si>
     <t>DANH SÁCH CÁC THUỘC TÍNH KIỂU DỮ LIỆU List</t>
@@ -500,13 +550,65 @@
     <t>Lưu thông tin tìm kiếm</t>
   </si>
   <si>
+    <t>getRepeaterId()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lấy mã lặp của task </t>
+  </si>
+  <si>
     <t>Lưu số lượng task trong danh sách</t>
+  </si>
+  <si>
+    <t>setTaskBeginDate()</t>
+  </si>
+  <si>
+    <t>Date taskBeginDate</t>
+  </si>
+  <si>
+    <t>Gán ngày bắt đầu của task cho task</t>
+  </si>
+  <si>
+    <t>viewTask</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int </t>
   </si>
   <si>
     <t>Lưu giao diện xem</t>
   </si>
   <si>
+    <t>0 : Xem dạng List
+1 : Xem dạng Board</t>
+  </si>
+  <si>
+    <t>getTaskBeginDate()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lấy ngày bắt đầu của task </t>
+  </si>
+  <si>
+    <t>taskStatusId</t>
+  </si>
+  <si>
+    <t>Lưu task có xóa hay không</t>
+  </si>
+  <si>
+    <t>setTaskEndDate()</t>
+  </si>
+  <si>
+    <t>Date taskEndDate</t>
+  </si>
+  <si>
+    <t>Gán ngày kết thúc của task cho task</t>
+  </si>
+  <si>
     <t>DANH SÁCH CÁC THUỘC TÍNH KIỂU DỮ LIỆU Date</t>
+  </si>
+  <si>
+    <t>getTaskEndDate()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lấy ngày kết thúc của task </t>
   </si>
   <si>
     <t>Ngày hiện tại</t>
@@ -516,7 +618,52 @@
 Ngày tháng nắm</t>
   </si>
   <si>
+    <t>setTaskFavoriteStatus()</t>
+  </si>
+  <si>
+    <t>boolean taskFavoriteStatus</t>
+  </si>
+  <si>
+    <t>Gán trạng thái yêu thích cho task</t>
+  </si>
+  <si>
+    <t>getTaskFavoriteStatus()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lấy trạng thái yêu thích của task </t>
+  </si>
+  <si>
+    <t>setTaskLate()</t>
+  </si>
+  <si>
+    <t>boolean taskLate</t>
+  </si>
+  <si>
+    <t>Gán trạng thái trễ hạn cho task</t>
+  </si>
+  <si>
+    <t>getTaskLate()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lấy trạng tháitrễ hạn của task </t>
+  </si>
+  <si>
+    <t>setTaskStatus()</t>
+  </si>
+  <si>
+    <t>int taskStatus</t>
+  </si>
+  <si>
+    <t>Gán trạng thái cho task</t>
+  </si>
+  <si>
     <t>DANH SÁCH CÁC THUỘC TÍNH KIỂU DỮ LIỆU Boolean</t>
+  </si>
+  <si>
+    <t>getTaskStatus()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lấy trạng thái của task </t>
   </si>
   <si>
     <t xml:space="preserve">false </t>
@@ -526,8 +673,14 @@
 false là không đánh dấu</t>
   </si>
   <si>
+    <t>Truyền thông tin sửa task controller từ xuống CSDL</t>
+  </si>
+  <si>
     <t>true là đã quá hạn
 false là vẫn chưa quá hạn</t>
+  </si>
+  <si>
+    <t>Thay đổi thông tin task dưới CSDL</t>
   </si>
   <si>
     <t xml:space="preserve">true </t>
@@ -536,6 +689,87 @@
     <t>true là không xóa
 false là xóa mềm</t>
   </si>
+  <si>
+    <t>deleteTask()</t>
+  </si>
+  <si>
+    <t>Lấy Id của task truyền xuống cotroller</t>
+  </si>
+  <si>
+    <t>Truyền Id của task từ view đến CSDL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Xóa task đã có dưới CSDL</t>
+  </si>
+  <si>
+    <t>sortTask()</t>
+  </si>
+  <si>
+    <t>String infoSort</t>
+  </si>
+  <si>
+    <t>Truyền thông tin sắp  xếp xuống controller và nhận danh sách task đã sắp xếp</t>
+  </si>
+  <si>
+    <t>Quick Sort</t>
+  </si>
+  <si>
+    <t>Sắp xếp theo tiêu chí và trả danh sách task lên view</t>
+  </si>
+  <si>
+    <t>groupByTask()</t>
+  </si>
+  <si>
+    <t>String infoGroupBy</t>
+  </si>
+  <si>
+    <t>Truyền thông tin gom nhóm xuống controller và nhận danh sách task đã gom nhóm</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>Gom nhóm theo tiêu chí và trả danh sách task lên view</t>
+  </si>
+  <si>
+    <t>regexTask()</t>
+  </si>
+  <si>
+    <t>String infoRegex</t>
+  </si>
+  <si>
+    <t>Truyền biểu thức chính quy xuống controller và nhận danh sách task đã tìm kiếm được</t>
+  </si>
+  <si>
+    <t>Tìm kiếm theo biểu thức chính quy và trả danh sách task lên view</t>
+  </si>
+  <si>
+    <t>searchTask()</t>
+  </si>
+  <si>
+    <t>String infoSearch</t>
+  </si>
+  <si>
+    <t>Truyền thông tin tìm kiếm xuống controller và nhận danh sách task đã tìm kiếm</t>
+  </si>
+  <si>
+    <t>Tìm kiếm theo thông tin và trả danh sách task lên view</t>
+  </si>
+  <si>
+    <t>completeTask()</t>
+  </si>
+  <si>
+    <t>Đánh dấu task hoàn thành</t>
+  </si>
+  <si>
+    <t>viewTask()</t>
+  </si>
+  <si>
+    <t>int viewTask</t>
+  </si>
+  <si>
+    <t>Chế độ xem dạng List hoặc Board</t>
+  </si>
 </sst>
 </file>
 
@@ -543,8 +777,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="26">
@@ -594,31 +828,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -630,16 +842,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -653,17 +858,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -678,7 +881,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -686,9 +896,17 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -708,9 +926,39 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -718,20 +966,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -746,7 +980,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -758,7 +1040,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -770,19 +1082,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -794,7 +1136,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -806,73 +1154,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -882,56 +1164,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1009,26 +1243,52 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1044,41 +1304,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1106,12 +1331,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1129,147 +1389,148 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1278,10 +1539,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1290,36 +1548,41 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1641,8 +1904,8 @@
   <sheetPr/>
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="W45" workbookViewId="0">
+      <selection activeCell="AF6" sqref="AF6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1"/>
@@ -1661,7 +1924,8 @@
     <col min="16" max="16" width="23.1428571428571" style="1" customWidth="1"/>
     <col min="17" max="22" width="14.4285714285714" style="1"/>
     <col min="23" max="23" width="20" style="1" customWidth="1"/>
-    <col min="24" max="27" width="14.4285714285714" style="1"/>
+    <col min="24" max="26" width="14.4285714285714" style="1"/>
+    <col min="27" max="27" width="19.8571428571429" style="1" customWidth="1"/>
     <col min="28" max="28" width="27.2857142857143" style="1" customWidth="1"/>
     <col min="29" max="30" width="14.4285714285714" style="1"/>
     <col min="31" max="31" width="18.2857142857143" style="1" customWidth="1"/>
@@ -1763,36 +2027,36 @@
         <v>8</v>
       </c>
       <c r="Y2" s="3"/>
-      <c r="Z2" s="23" t="s">
+      <c r="Z2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="AA2" s="23" t="s">
+      <c r="AA2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="AB2" s="23" t="s">
+      <c r="AB2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="AC2" s="23" t="s">
+      <c r="AC2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="AD2" s="23" t="s">
+      <c r="AD2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="AE2" s="23" t="s">
+      <c r="AE2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="AF2" s="23" t="s">
+      <c r="AF2" s="18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="25.5" spans="1:32">
+    <row r="3" s="1" customFormat="1" ht="51" spans="1:32">
       <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="5"/>
@@ -1806,13 +2070,13 @@
       <c r="H3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="5"/>
+      <c r="I3" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="J3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="K3" s="5"/>
       <c r="L3" s="3"/>
       <c r="M3" s="5">
         <v>1</v>
@@ -1823,10 +2087,10 @@
       <c r="O3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="6"/>
+      <c r="Q3" s="5"/>
       <c r="R3" s="3"/>
       <c r="S3" s="5">
         <v>1</v>
@@ -1840,30 +2104,30 @@
       <c r="V3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="W3" s="5" t="s">
         <v>29</v>
       </c>
       <c r="X3" s="5"/>
       <c r="Y3" s="3"/>
-      <c r="Z3" s="10">
+      <c r="Z3" s="8">
         <v>1</v>
       </c>
-      <c r="AA3" s="11" t="s">
+      <c r="AA3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="AB3" s="11" t="s">
+      <c r="AB3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AC3" s="11" t="s">
+      <c r="AC3" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="AD3" s="11" t="s">
+      <c r="AD3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AE3" s="11" t="s">
+      <c r="AE3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AF3" s="11"/>
+      <c r="AF3" s="9"/>
     </row>
     <row r="4" s="1" customFormat="1" ht="123.75" spans="1:32">
       <c r="A4" s="5">
@@ -1872,7 +2136,7 @@
       <c r="B4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D4" s="5"/>
@@ -1886,11 +2150,11 @@
       <c r="H4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>38</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="3"/>
@@ -1903,52 +2167,56 @@
       <c r="O4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q4" s="6"/>
+      <c r="P4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q4" s="5"/>
       <c r="R4" s="3"/>
       <c r="S4" s="5">
         <v>2</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="U4" s="5" t="s">
         <v>23</v>
       </c>
       <c r="V4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="W4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="W4" s="6" t="s">
+      <c r="X4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="X4" s="6" t="s">
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="9">
+        <v>2</v>
+      </c>
+      <c r="AA4" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="10">
-        <v>2</v>
-      </c>
-      <c r="AA4" s="11" t="s">
+      <c r="AB4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE4" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="AB4" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="11"/>
-      <c r="AE4" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF4" s="11"/>
-    </row>
-    <row r="5" s="1" customFormat="1" ht="76.5" spans="1:32">
+      <c r="AF4" s="9"/>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="63.75" spans="1:32">
       <c r="A5" s="5">
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -1957,75 +2225,77 @@
         <v>3</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>51</v>
+        <v>25</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="5">
         <v>3</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q5" s="6"/>
+      <c r="P5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q5" s="5"/>
       <c r="R5" s="3"/>
       <c r="S5" s="5">
         <v>3</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="U5" s="5" t="s">
         <v>23</v>
       </c>
       <c r="V5" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="W5" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="X5" s="5"/>
       <c r="Y5" s="3"/>
-      <c r="Z5" s="10">
+      <c r="Z5" s="9">
         <v>3</v>
       </c>
-      <c r="AA5" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB5" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC5" s="11"/>
-      <c r="AD5" s="11"/>
-      <c r="AE5" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF5" s="11"/>
+      <c r="AA5" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD5" s="9"/>
+      <c r="AE5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF5" s="9"/>
     </row>
     <row r="6" s="1" customFormat="1" ht="38.25" spans="1:32">
       <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="3"/>
@@ -2033,14 +2303,14 @@
         <v>4</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="3"/>
@@ -2048,58 +2318,58 @@
         <v>4</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="O6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="P6" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q6" s="6"/>
+      <c r="P6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q6" s="5"/>
       <c r="R6" s="3"/>
       <c r="S6" s="5">
         <v>4</v>
       </c>
       <c r="T6" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="U6" s="5" t="s">
         <v>23</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="W6" s="6" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="W6" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="X6" s="5"/>
       <c r="Y6" s="3"/>
-      <c r="Z6" s="10">
+      <c r="Z6" s="9">
         <v>4</v>
       </c>
-      <c r="AA6" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB6" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC6" s="11"/>
-      <c r="AD6" s="11"/>
-      <c r="AE6" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF6" s="11"/>
+      <c r="AA6" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF6" s="9"/>
     </row>
     <row r="7" s="1" customFormat="1" ht="26.25" customHeight="1" spans="1:32">
       <c r="A7" s="5">
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>70</v>
+        <v>64</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="3"/>
@@ -2107,14 +2377,14 @@
         <v>5</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="3"/>
@@ -2122,79 +2392,76 @@
         <v>5</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="O7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="P7" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q7" s="6"/>
+      <c r="P7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q7" s="5"/>
       <c r="R7" s="3"/>
       <c r="S7" s="5">
         <v>5</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="U7" s="5" t="s">
         <v>23</v>
       </c>
       <c r="V7" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="W7" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
+      </c>
+      <c r="W7" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="X7" s="5"/>
       <c r="Y7" s="3"/>
-      <c r="Z7" s="10">
+      <c r="Z7" s="8">
         <v>5</v>
       </c>
-      <c r="AA7" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="AB7" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC7" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD7" s="11"/>
-      <c r="AE7" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF7" s="11"/>
+      <c r="AA7" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB7" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF7" s="9"/>
     </row>
     <row r="8" s="1" customFormat="1" ht="38.25" spans="1:32">
       <c r="A8" s="5">
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>81</v>
+        <v>75</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="5">
         <v>6</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="6" t="s">
-        <v>83</v>
+      <c r="I8" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="3"/>
@@ -2202,278 +2469,278 @@
         <v>6</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="O8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="P8" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q8" s="6"/>
+      <c r="P8" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q8" s="5"/>
       <c r="R8" s="3"/>
       <c r="S8" s="5">
         <v>6</v>
       </c>
       <c r="T8" s="5" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="U8" s="5" t="s">
         <v>23</v>
       </c>
       <c r="V8" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="W8" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
+      </c>
+      <c r="W8" s="5" t="s">
+        <v>82</v>
       </c>
       <c r="X8" s="5"/>
       <c r="Y8" s="3"/>
-      <c r="Z8" s="10">
+      <c r="Z8" s="9">
         <v>6</v>
       </c>
-      <c r="AA8" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB8" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="AC8" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD8" s="11"/>
-      <c r="AE8" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AF8" s="11"/>
+      <c r="AA8" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB8" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC8" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD8" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE8" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF8" s="9"/>
     </row>
     <row r="9" s="1" customFormat="1" ht="38.25" spans="1:32">
       <c r="A9" s="5">
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <v>7</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="H9" s="8" t="s">
+      <c r="G9" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="K9" s="8"/>
+      <c r="I9" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="7"/>
       <c r="L9" s="3"/>
       <c r="M9" s="5">
         <v>7</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="O9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="P9" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q9" s="6"/>
+      <c r="P9" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q9" s="5"/>
       <c r="R9" s="3"/>
       <c r="S9" s="5">
         <v>7</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="U9" s="5" t="s">
         <v>23</v>
       </c>
       <c r="V9" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="W9" s="6" t="s">
-        <v>97</v>
+        <v>90</v>
+      </c>
+      <c r="W9" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="X9" s="5"/>
       <c r="Y9" s="3"/>
-      <c r="Z9" s="10">
+      <c r="Z9" s="9">
         <v>7</v>
       </c>
-      <c r="AA9" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="AB9" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="AC9" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD9" s="11"/>
-      <c r="AE9" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="AF9" s="11"/>
+      <c r="AA9" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB9" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF9" s="9"/>
     </row>
     <row r="10" s="1" customFormat="1" ht="38.25" spans="1:32">
       <c r="A10" s="5">
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <v>8</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="H10" s="9" t="s">
+      <c r="G10" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="K10" s="9"/>
+      <c r="I10" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" s="8"/>
       <c r="L10" s="3"/>
       <c r="M10" s="5">
         <v>8</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="O10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="P10" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q10" s="6"/>
+      <c r="P10" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q10" s="5"/>
       <c r="R10" s="3"/>
-      <c r="S10" s="8">
+      <c r="S10" s="7">
         <v>9</v>
       </c>
-      <c r="T10" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="U10" s="8" t="s">
+      <c r="T10" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="V10" s="8">
+      <c r="V10" s="7">
         <v>1000</v>
       </c>
-      <c r="W10" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="X10" s="8"/>
+      <c r="W10" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="X10" s="7"/>
       <c r="Y10" s="3"/>
-      <c r="Z10" s="10">
+      <c r="Z10" s="9">
         <v>8</v>
       </c>
-      <c r="AA10" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="AB10" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="AC10" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD10" s="11"/>
-      <c r="AE10" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="AF10" s="11"/>
+      <c r="AA10" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB10" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC10" s="9"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF10" s="9"/>
     </row>
     <row r="11" s="1" customFormat="1" ht="26.25" customHeight="1" spans="1:32">
       <c r="A11" s="5">
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>111</v>
+        <v>101</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="10">
+      <c r="F11" s="8">
         <v>9</v>
       </c>
-      <c r="G11" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="H11" s="10" t="s">
+      <c r="G11" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="H11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="K11" s="10"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="8"/>
       <c r="L11" s="3"/>
       <c r="M11" s="5">
         <v>9</v>
       </c>
-      <c r="N11" s="8" t="s">
-        <v>113</v>
+      <c r="N11" s="7" t="s">
+        <v>104</v>
       </c>
       <c r="O11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="P11" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q11" s="6"/>
+      <c r="P11" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q11" s="5"/>
       <c r="R11" s="3"/>
-      <c r="S11" s="9">
+      <c r="S11" s="8">
         <v>10</v>
       </c>
-      <c r="T11" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="U11" s="9" t="s">
+      <c r="T11" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="U11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="V11" s="9">
+      <c r="V11" s="8">
         <v>5</v>
       </c>
-      <c r="W11" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="X11" s="9"/>
+      <c r="W11" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="X11" s="8"/>
       <c r="Y11" s="3"/>
-      <c r="Z11" s="10">
+      <c r="Z11" s="9">
         <v>9</v>
       </c>
-      <c r="AA11" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB11" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="AC11" s="11"/>
-      <c r="AD11" s="11"/>
-      <c r="AE11" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="AF11" s="11"/>
-    </row>
-    <row r="12" s="1" customFormat="1" ht="26.25" customHeight="1" spans="1:32">
+      <c r="AA11" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB11" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF11" s="9"/>
+    </row>
+    <row r="12" s="1" customFormat="1" ht="25.5" spans="1:32">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -2481,107 +2748,115 @@
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="11">
+      <c r="F12" s="9">
         <v>10</v>
       </c>
-      <c r="G12" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="H12" s="11" t="s">
+      <c r="G12" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="H12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="K12" s="11"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="9"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="15">
+      <c r="M12" s="12">
         <v>10</v>
       </c>
-      <c r="N12" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="O12" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="P12" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q12" s="6"/>
+      <c r="N12" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="O12" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q12" s="5"/>
       <c r="R12" s="3"/>
-      <c r="S12" s="12"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="12"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="12"/>
-      <c r="X12" s="12"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
       <c r="Y12" s="3"/>
-      <c r="Z12" s="10">
+      <c r="Z12" s="8">
         <v>10</v>
       </c>
-      <c r="AA12" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="AB12" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC12" s="11"/>
-      <c r="AD12" s="11"/>
-      <c r="AE12" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="AF12" s="11"/>
-    </row>
-    <row r="13" s="1" customFormat="1" ht="26.25" customHeight="1" spans="1:32">
+      <c r="AA12" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB12" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF12" s="9"/>
+    </row>
+    <row r="13" s="1" customFormat="1" ht="76.5" spans="1:32">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="11">
+      <c r="F13" s="9">
         <v>11</v>
       </c>
-      <c r="G13" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="H13" s="11" t="s">
+      <c r="G13" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="K13" s="11"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" s="9"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="15">
+      <c r="M13" s="12">
         <v>11</v>
       </c>
-      <c r="N13" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="O13" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="P13" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q13" s="6"/>
+      <c r="N13" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="O13" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q13" s="5"/>
       <c r="R13" s="3"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="12"/>
-      <c r="W13" s="12"/>
-      <c r="X13" s="12"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
+      <c r="W13" s="10"/>
+      <c r="X13" s="10"/>
       <c r="Y13" s="3"/>
-      <c r="Z13" s="21"/>
-      <c r="AA13" s="24"/>
-      <c r="AB13" s="24"/>
-      <c r="AC13" s="24"/>
-      <c r="AD13" s="24"/>
-      <c r="AE13" s="24"/>
-      <c r="AF13" s="24"/>
+      <c r="Z13" s="9">
+        <v>11</v>
+      </c>
+      <c r="AA13" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB13" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC13" s="9"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF13" s="9"/>
     </row>
     <row r="14" s="1" customFormat="1" ht="26.25" customHeight="1" spans="1:32">
       <c r="A14" s="3"/>
@@ -2589,91 +2864,103 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="11">
+      <c r="F14" s="9">
         <v>12</v>
       </c>
-      <c r="G14" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="H14" s="11" t="s">
+      <c r="G14" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="H14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="K14" s="11"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="9"/>
       <c r="L14" s="3"/>
       <c r="M14" s="5">
         <v>12</v>
       </c>
-      <c r="N14" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="O14" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="P14" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q14" s="6"/>
+      <c r="N14" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="O14" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q14" s="5"/>
       <c r="R14" s="3"/>
-      <c r="S14" s="21"/>
-      <c r="T14" s="21"/>
-      <c r="U14" s="21"/>
-      <c r="V14" s="21"/>
-      <c r="W14" s="21"/>
-      <c r="X14" s="21"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
+      <c r="V14" s="16"/>
+      <c r="W14" s="16"/>
+      <c r="X14" s="16"/>
       <c r="Y14" s="3"/>
-      <c r="Z14" s="21"/>
-      <c r="AA14" s="24"/>
-      <c r="AB14" s="24"/>
-      <c r="AC14" s="24"/>
-      <c r="AD14" s="24"/>
-      <c r="AE14" s="24"/>
-      <c r="AF14" s="24"/>
-    </row>
-    <row r="15" s="1" customFormat="1" ht="26.25" customHeight="1" spans="1:32">
+      <c r="Z14" s="9">
+        <v>12</v>
+      </c>
+      <c r="AA14" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB14" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC14" s="9"/>
+      <c r="AD14" s="9"/>
+      <c r="AE14" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="AF14" s="9"/>
+    </row>
+    <row r="15" s="1" customFormat="1" ht="25" customHeight="1" spans="1:32">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
       <c r="L15" s="3"/>
       <c r="M15" s="5">
         <v>13</v>
       </c>
-      <c r="N15" s="16" t="s">
+      <c r="N15" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="O15" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="16"/>
+      <c r="V15" s="16"/>
+      <c r="W15" s="16"/>
+      <c r="X15" s="16"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="9">
+        <v>13</v>
+      </c>
+      <c r="AA15" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB15" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC15" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD15" s="9"/>
+      <c r="AE15" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="O15" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="P15" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="21"/>
-      <c r="T15" s="21"/>
-      <c r="U15" s="21"/>
-      <c r="V15" s="21"/>
-      <c r="W15" s="21"/>
-      <c r="X15" s="21"/>
-      <c r="Y15" s="3"/>
-      <c r="Z15" s="21"/>
-      <c r="AA15" s="24"/>
-      <c r="AB15" s="24"/>
-      <c r="AC15" s="24"/>
-      <c r="AD15" s="24"/>
-      <c r="AE15" s="24"/>
-      <c r="AF15" s="24"/>
+      <c r="AF15" s="9"/>
     </row>
     <row r="16" s="1" customFormat="1" ht="26.25" customHeight="1" spans="1:32">
       <c r="A16" s="3"/>
@@ -2682,181 +2969,213 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L16" s="3"/>
       <c r="M16" s="5">
         <v>14</v>
       </c>
       <c r="N16" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="O16" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="O16" s="5" t="s">
+      <c r="P16" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="P16" s="6" t="s">
+      <c r="Q16" s="5"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
+      <c r="V16" s="16"/>
+      <c r="W16" s="16"/>
+      <c r="X16" s="16"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="9">
+        <v>14</v>
+      </c>
+      <c r="AA16" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="21"/>
-      <c r="T16" s="21"/>
-      <c r="U16" s="21"/>
-      <c r="V16" s="21"/>
-      <c r="W16" s="21"/>
-      <c r="X16" s="21"/>
-      <c r="Y16" s="3"/>
-      <c r="Z16" s="21"/>
-      <c r="AA16" s="24"/>
-      <c r="AB16" s="24"/>
-      <c r="AC16" s="24"/>
-      <c r="AD16" s="24"/>
-      <c r="AE16" s="24"/>
-      <c r="AF16" s="24"/>
-    </row>
-    <row r="17" s="1" customFormat="1" ht="26.25" customHeight="1" spans="1:32">
+      <c r="AB16" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC16" s="9"/>
+      <c r="AD16" s="9"/>
+      <c r="AE16" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="AF16" s="9"/>
+    </row>
+    <row r="17" s="1" customFormat="1" ht="25.5" spans="1:32">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="11">
+      <c r="F17" s="9">
         <v>1</v>
       </c>
-      <c r="G17" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="H17" s="11" t="s">
+      <c r="G17" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11">
+      <c r="I17" s="9"/>
+      <c r="J17" s="9">
         <v>0</v>
       </c>
-      <c r="K17" s="19"/>
+      <c r="K17" s="15"/>
       <c r="L17" s="3"/>
       <c r="M17" s="5">
         <v>15</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="P17" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q17" s="6"/>
+        <v>64</v>
+      </c>
+      <c r="P17" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q17" s="5"/>
       <c r="R17" s="3"/>
-      <c r="S17" s="21"/>
-      <c r="T17" s="21"/>
-      <c r="U17" s="21"/>
-      <c r="V17" s="21"/>
-      <c r="W17" s="21"/>
-      <c r="X17" s="21"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
+      <c r="V17" s="16"/>
+      <c r="W17" s="16"/>
+      <c r="X17" s="16"/>
       <c r="Y17" s="3"/>
-      <c r="Z17" s="21"/>
-      <c r="AA17" s="24"/>
-      <c r="AB17" s="24"/>
-      <c r="AC17" s="24"/>
-      <c r="AD17" s="24"/>
-      <c r="AE17" s="24"/>
-      <c r="AF17" s="24"/>
-    </row>
-    <row r="18" s="1" customFormat="1" ht="26.25" customHeight="1" spans="1:32">
+      <c r="Z17" s="8">
+        <v>15</v>
+      </c>
+      <c r="AA17" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="AB17" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD17" s="9"/>
+      <c r="AE17" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF17" s="15"/>
+    </row>
+    <row r="18" s="1" customFormat="1" ht="38.25" spans="1:32">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="11">
+      <c r="F18" s="8">
         <v>2</v>
       </c>
-      <c r="G18" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11">
+      <c r="G18" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8">
         <v>0</v>
       </c>
-      <c r="K18" s="11" t="s">
-        <v>142</v>
+      <c r="K18" s="8" t="s">
+        <v>145</v>
       </c>
       <c r="L18" s="3"/>
-      <c r="M18" s="8">
+      <c r="M18" s="7">
         <v>16</v>
       </c>
-      <c r="N18" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="O18" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="P18" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q18" s="18"/>
+      <c r="N18" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="O18" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="P18" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q18" s="7"/>
       <c r="R18" s="3"/>
-      <c r="S18" s="21"/>
-      <c r="T18" s="21"/>
-      <c r="U18" s="21"/>
-      <c r="V18" s="21"/>
-      <c r="W18" s="21"/>
-      <c r="X18" s="21"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="16"/>
+      <c r="U18" s="16"/>
+      <c r="V18" s="16"/>
+      <c r="W18" s="16"/>
+      <c r="X18" s="16"/>
       <c r="Y18" s="3"/>
-      <c r="Z18" s="21"/>
-      <c r="AA18" s="24"/>
-      <c r="AB18" s="24"/>
-      <c r="AC18" s="24"/>
-      <c r="AD18" s="24"/>
-      <c r="AE18" s="24"/>
-      <c r="AF18" s="24"/>
-    </row>
-    <row r="19" s="1" customFormat="1" ht="27" customHeight="1" spans="1:32">
+      <c r="Z18" s="9">
+        <v>16</v>
+      </c>
+      <c r="AA18" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="AB18" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="AC18" s="9"/>
+      <c r="AD18" s="9"/>
+      <c r="AE18" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="AF18" s="9"/>
+    </row>
+    <row r="19" s="1" customFormat="1" ht="51" spans="1:32">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="9">
+      <c r="M19" s="8">
         <v>17</v>
       </c>
-      <c r="N19" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="O19" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="P19" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="Q19" s="10"/>
+      <c r="N19" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="O19" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P19" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q19" s="8" t="s">
+        <v>152</v>
+      </c>
       <c r="R19" s="3"/>
-      <c r="S19" s="21"/>
-      <c r="T19" s="21"/>
-      <c r="U19" s="21"/>
-      <c r="V19" s="21"/>
-      <c r="W19" s="21"/>
-      <c r="X19" s="21"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
+      <c r="U19" s="16"/>
+      <c r="V19" s="16"/>
+      <c r="W19" s="16"/>
+      <c r="X19" s="16"/>
       <c r="Y19" s="3"/>
-      <c r="Z19" s="21"/>
-      <c r="AA19" s="24"/>
-      <c r="AB19" s="24"/>
-      <c r="AC19" s="24"/>
-      <c r="AD19" s="24"/>
-      <c r="AE19" s="24"/>
-      <c r="AF19" s="24"/>
+      <c r="Z19" s="9">
+        <v>17</v>
+      </c>
+      <c r="AA19" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB19" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD19" s="9"/>
+      <c r="AE19" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="AF19" s="15"/>
     </row>
     <row r="20" s="1" customFormat="1" ht="27" customHeight="1" spans="1:32">
       <c r="A20" s="3"/>
@@ -2865,37 +3184,45 @@
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="2" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="L20" s="3"/>
-      <c r="M20" s="11">
+      <c r="M20" s="9">
         <v>18</v>
       </c>
-      <c r="N20" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="O20" s="11" t="s">
+      <c r="N20" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="O20" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="P20" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q20" s="10"/>
+      <c r="P20" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q20" s="8"/>
       <c r="R20" s="3"/>
-      <c r="S20" s="21"/>
-      <c r="T20" s="21"/>
-      <c r="U20" s="21"/>
-      <c r="V20" s="21"/>
-      <c r="W20" s="21"/>
-      <c r="X20" s="21"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="16"/>
+      <c r="V20" s="16"/>
+      <c r="W20" s="16"/>
+      <c r="X20" s="16"/>
       <c r="Y20" s="3"/>
-      <c r="Z20" s="21"/>
-      <c r="AA20" s="24"/>
-      <c r="AB20" s="24"/>
-      <c r="AC20" s="24"/>
-      <c r="AD20" s="24"/>
-      <c r="AE20" s="24"/>
-      <c r="AF20" s="24"/>
+      <c r="Z20" s="9">
+        <v>18</v>
+      </c>
+      <c r="AA20" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="AB20" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="AC20" s="9"/>
+      <c r="AD20" s="9"/>
+      <c r="AE20" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="AF20" s="9"/>
     </row>
     <row r="21" s="1" customFormat="1" ht="27" customHeight="1" spans="1:32">
       <c r="A21" s="3"/>
@@ -2907,32 +3234,32 @@
         <v>1</v>
       </c>
       <c r="G21" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="H21" s="5" t="s">
         <v>134</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>135</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>150</v>
+        <v>160</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>161</v>
       </c>
       <c r="L21" s="3"/>
-      <c r="M21" s="11">
+      <c r="M21" s="9">
         <v>19</v>
       </c>
-      <c r="N21" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="O21" s="11" t="s">
+      <c r="N21" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="O21" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="P21" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q21" s="10"/>
+      <c r="P21" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q21" s="8"/>
       <c r="R21" s="3"/>
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
@@ -2941,13 +3268,23 @@
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
       <c r="Y21" s="3"/>
-      <c r="Z21" s="21"/>
-      <c r="AA21" s="24"/>
-      <c r="AB21" s="24"/>
-      <c r="AC21" s="24"/>
-      <c r="AD21" s="24"/>
-      <c r="AE21" s="24"/>
-      <c r="AF21" s="24"/>
+      <c r="Z21" s="9">
+        <v>19</v>
+      </c>
+      <c r="AA21" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB21" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC21" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD21" s="9"/>
+      <c r="AE21" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="AF21" s="15"/>
     </row>
     <row r="22" s="1" customFormat="1" ht="27" customHeight="1" spans="1:32">
       <c r="A22" s="3"/>
@@ -2955,26 +3292,26 @@
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
       <c r="L22" s="3"/>
-      <c r="M22" s="11">
+      <c r="M22" s="9">
         <v>20</v>
       </c>
-      <c r="N22" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="O22" s="11" t="s">
+      <c r="N22" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="O22" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="P22" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q22" s="10"/>
+      <c r="P22" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q22" s="8"/>
       <c r="R22" s="3"/>
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
@@ -2983,13 +3320,21 @@
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
       <c r="Y22" s="3"/>
-      <c r="Z22" s="21"/>
-      <c r="AA22" s="24"/>
-      <c r="AB22" s="24"/>
-      <c r="AC22" s="24"/>
-      <c r="AD22" s="24"/>
-      <c r="AE22" s="24"/>
-      <c r="AF22" s="24"/>
+      <c r="Z22" s="8">
+        <v>20</v>
+      </c>
+      <c r="AA22" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB22" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="AC22" s="9"/>
+      <c r="AD22" s="9"/>
+      <c r="AE22" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="AF22" s="9"/>
     </row>
     <row r="23" s="1" customFormat="1" ht="27" customHeight="1" spans="1:32">
       <c r="A23" s="3"/>
@@ -2998,22 +3343,22 @@
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="2" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="L23" s="3"/>
-      <c r="M23" s="10">
+      <c r="M23" s="8">
         <v>21</v>
       </c>
-      <c r="N23" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="O23" s="10" t="s">
+      <c r="N23" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="O23" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="P23" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q23" s="22"/>
+      <c r="P23" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q23" s="17"/>
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
@@ -3022,52 +3367,62 @@
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
       <c r="Y23" s="3"/>
-      <c r="Z23" s="21"/>
-      <c r="AA23" s="24"/>
-      <c r="AB23" s="24"/>
-      <c r="AC23" s="24"/>
-      <c r="AD23" s="24"/>
-      <c r="AE23" s="24"/>
-      <c r="AF23" s="24"/>
-    </row>
-    <row r="24" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z23" s="9">
+        <v>21</v>
+      </c>
+      <c r="AA23" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB23" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC23" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD23" s="9"/>
+      <c r="AE23" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="AF23" s="15"/>
+    </row>
+    <row r="24" s="1" customFormat="1" ht="27" customHeight="1" spans="1:32">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H24" s="13" t="s">
+      <c r="H24" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="I24" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J24" s="13" t="s">
+      <c r="J24" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="K24" s="13" t="s">
+      <c r="K24" s="11" t="s">
         <v>8</v>
       </c>
       <c r="L24" s="3"/>
-      <c r="M24" s="11">
+      <c r="M24" s="9">
         <v>22</v>
       </c>
-      <c r="N24" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="O24" s="11" t="s">
+      <c r="N24" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="O24" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="P24" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q24" s="10"/>
+      <c r="P24" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q24" s="8"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
@@ -3076,42 +3431,58 @@
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
       <c r="Y24" s="3"/>
-      <c r="Z24" s="3"/>
-    </row>
-    <row r="25" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z24" s="9">
+        <v>22</v>
+      </c>
+      <c r="AA24" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="AB24" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="AC24" s="9"/>
+      <c r="AD24" s="9"/>
+      <c r="AE24" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="AF24" s="9"/>
+    </row>
+    <row r="25" s="1" customFormat="1" ht="38.25" spans="1:32">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="9">
+      <c r="F25" s="8">
         <v>1</v>
       </c>
-      <c r="G25" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="H25" s="9" t="s">
+      <c r="G25" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H25" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="K25" s="9"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K25" s="8"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="11">
+      <c r="M25" s="9">
         <v>23</v>
       </c>
-      <c r="N25" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="O25" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="P25" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q25" s="10"/>
+      <c r="N25" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="O25" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="P25" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q25" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
@@ -3120,26 +3491,44 @@
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
       <c r="Y25" s="3"/>
-      <c r="Z25" s="3"/>
-    </row>
-    <row r="26" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z25" s="9">
+        <v>23</v>
+      </c>
+      <c r="AA25" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB25" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC25" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD25" s="9"/>
+      <c r="AE25" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="AF25" s="15"/>
+    </row>
+    <row r="26" s="1" customFormat="1" ht="27" customHeight="1" spans="1:32">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="20"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="21"/>
-      <c r="N26" s="21"/>
-      <c r="O26" s="21"/>
-      <c r="P26" s="21"/>
-      <c r="Q26" s="21"/>
+      <c r="M26" s="8">
+        <v>24</v>
+      </c>
+      <c r="N26" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="O26" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="P26" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q26" s="8"/>
       <c r="R26" s="3"/>
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
@@ -3148,23 +3537,37 @@
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
       <c r="Y26" s="3"/>
-      <c r="Z26" s="3"/>
-    </row>
-    <row r="27" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z26" s="9">
+        <v>24</v>
+      </c>
+      <c r="AA26" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="AB26" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC26" s="9"/>
+      <c r="AD26" s="9"/>
+      <c r="AE26" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="AF26" s="9"/>
+    </row>
+    <row r="27" s="1" customFormat="1" ht="25.5" spans="1:32">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="2" t="s">
-        <v>157</v>
+        <v>188</v>
       </c>
       <c r="L27" s="3"/>
-      <c r="M27" s="21"/>
-      <c r="N27" s="21"/>
-      <c r="O27" s="21"/>
-      <c r="P27" s="21"/>
-      <c r="Q27" s="21"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
@@ -3173,74 +3576,103 @@
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
       <c r="Y27" s="3"/>
-      <c r="Z27" s="3"/>
-    </row>
-    <row r="28" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z27" s="8">
+        <v>25</v>
+      </c>
+      <c r="AA27" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="AB27" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC27" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD27" s="9"/>
+      <c r="AE27" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="AF27" s="15"/>
+    </row>
+    <row r="28" s="1" customFormat="1" ht="27" customHeight="1" spans="1:32">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="15">
+      <c r="F28" s="12">
         <v>1</v>
       </c>
-      <c r="G28" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="H28" s="17" t="s">
-        <v>110</v>
+      <c r="G28" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="I28" s="5"/>
       <c r="J28" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>159</v>
+        <v>191</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>192</v>
       </c>
       <c r="L28" s="3"/>
-      <c r="M28" s="21"/>
-      <c r="N28" s="21"/>
-      <c r="O28" s="21"/>
-      <c r="P28" s="21"/>
-      <c r="Q28" s="21"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
-      <c r="X28" s="3"/>
       <c r="Y28" s="3"/>
-      <c r="Z28" s="3"/>
-    </row>
-    <row r="29" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z28" s="9">
+        <v>26</v>
+      </c>
+      <c r="AA28" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="AB28" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC28" s="9"/>
+      <c r="AD28" s="9"/>
+      <c r="AE28" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="AF28" s="9"/>
+    </row>
+    <row r="29" s="1" customFormat="1" ht="27" customHeight="1" spans="1:32">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="15">
+      <c r="F29" s="12">
         <v>2</v>
       </c>
-      <c r="G29" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="H29" s="17" t="s">
-        <v>110</v>
+      <c r="G29" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="I29" s="5"/>
       <c r="J29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>159</v>
+        <v>25</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>192</v>
       </c>
       <c r="L29" s="3"/>
-      <c r="M29" s="21"/>
-      <c r="N29" s="21"/>
-      <c r="O29" s="21"/>
-      <c r="P29" s="21"/>
-      <c r="Q29" s="21"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
       <c r="R29" s="3"/>
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
@@ -3249,36 +3681,52 @@
       <c r="W29" s="3"/>
       <c r="X29" s="3"/>
       <c r="Y29" s="3"/>
-      <c r="Z29" s="3"/>
-    </row>
-    <row r="30" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z29" s="9">
+        <v>27</v>
+      </c>
+      <c r="AA29" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="AB29" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC29" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD29" s="9"/>
+      <c r="AE29" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF29" s="15"/>
+    </row>
+    <row r="30" s="1" customFormat="1" ht="27" customHeight="1" spans="1:32">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="15">
+      <c r="F30" s="12">
         <v>3</v>
       </c>
-      <c r="G30" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="H30" s="17" t="s">
-        <v>110</v>
+      <c r="G30" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="I30" s="5"/>
       <c r="J30" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="K30" s="6" t="s">
-        <v>159</v>
+        <v>191</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>192</v>
       </c>
       <c r="L30" s="3"/>
-      <c r="M30" s="21"/>
-      <c r="N30" s="21"/>
-      <c r="O30" s="21"/>
-      <c r="P30" s="21"/>
-      <c r="Q30" s="21"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
       <c r="R30" s="3"/>
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
@@ -3287,36 +3735,50 @@
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
       <c r="Y30" s="3"/>
-      <c r="Z30" s="3"/>
-    </row>
-    <row r="31" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z30" s="9">
+        <v>28</v>
+      </c>
+      <c r="AA30" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="AB30" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="AC30" s="9"/>
+      <c r="AD30" s="9"/>
+      <c r="AE30" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="AF30" s="9"/>
+    </row>
+    <row r="31" s="1" customFormat="1" ht="27" customHeight="1" spans="1:32">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="15">
+      <c r="F31" s="12">
         <v>4</v>
       </c>
-      <c r="G31" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="H31" s="17" t="s">
-        <v>110</v>
+      <c r="G31" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="I31" s="5"/>
       <c r="J31" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>159</v>
+        <v>25</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>192</v>
       </c>
       <c r="L31" s="3"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21"/>
-      <c r="O31" s="21"/>
-      <c r="P31" s="21"/>
-      <c r="Q31" s="21"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
       <c r="R31" s="3"/>
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
@@ -3325,26 +3787,36 @@
       <c r="W31" s="3"/>
       <c r="X31" s="3"/>
       <c r="Y31" s="3"/>
-      <c r="Z31" s="3"/>
-    </row>
-    <row r="32" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z31" s="9">
+        <v>29</v>
+      </c>
+      <c r="AA31" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB31" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC31" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD31" s="9"/>
+      <c r="AE31" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="AF31" s="15"/>
+    </row>
+    <row r="32" s="1" customFormat="1" ht="27" customHeight="1" spans="1:32">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
       <c r="L32" s="3"/>
-      <c r="M32" s="21"/>
-      <c r="N32" s="21"/>
-      <c r="O32" s="21"/>
-      <c r="P32" s="21"/>
-      <c r="Q32" s="21"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="16"/>
       <c r="R32" s="3"/>
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
@@ -3353,23 +3825,37 @@
       <c r="W32" s="3"/>
       <c r="X32" s="3"/>
       <c r="Y32" s="3"/>
-      <c r="Z32" s="3"/>
-    </row>
-    <row r="33" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z32" s="8">
+        <v>30</v>
+      </c>
+      <c r="AA32" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AB32" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="AC32" s="9"/>
+      <c r="AD32" s="9"/>
+      <c r="AE32" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="AF32" s="9"/>
+    </row>
+    <row r="33" s="1" customFormat="1" ht="27" customHeight="1" spans="1:32">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="2" t="s">
-        <v>160</v>
+        <v>206</v>
       </c>
       <c r="L33" s="3"/>
-      <c r="M33" s="21"/>
-      <c r="N33" s="21"/>
-      <c r="O33" s="21"/>
-      <c r="P33" s="21"/>
-      <c r="Q33" s="21"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="16"/>
       <c r="R33" s="3"/>
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
@@ -3378,9 +3864,25 @@
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
       <c r="Y33" s="3"/>
-      <c r="Z33" s="3"/>
-    </row>
-    <row r="34" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z33" s="9">
+        <v>31</v>
+      </c>
+      <c r="AA33" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="AB33" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC33" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD33" s="9"/>
+      <c r="AE33" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="AF33" s="15"/>
+    </row>
+    <row r="34" s="1" customFormat="1" ht="76.5" spans="1:32">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -3390,24 +3892,24 @@
         <v>1</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="I34" s="5"/>
       <c r="J34" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="K34" s="6" t="s">
-        <v>162</v>
+        <v>209</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>210</v>
       </c>
       <c r="L34" s="3"/>
-      <c r="M34" s="21"/>
-      <c r="N34" s="21"/>
-      <c r="O34" s="21"/>
-      <c r="P34" s="21"/>
-      <c r="Q34" s="21"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
       <c r="R34" s="3"/>
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
@@ -3416,36 +3918,50 @@
       <c r="W34" s="3"/>
       <c r="X34" s="3"/>
       <c r="Y34" s="3"/>
-      <c r="Z34" s="3"/>
-    </row>
-    <row r="35" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z34" s="9">
+        <v>32</v>
+      </c>
+      <c r="AA34" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB34" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC34" s="9"/>
+      <c r="AD34" s="9"/>
+      <c r="AE34" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="AF34" s="9"/>
+    </row>
+    <row r="35" s="1" customFormat="1" ht="76.5" spans="1:32">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="8">
+      <c r="F35" s="7">
         <v>2</v>
       </c>
-      <c r="G35" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="H35" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="K35" s="18" t="s">
-        <v>163</v>
+      <c r="G35" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>212</v>
       </c>
       <c r="L35" s="3"/>
-      <c r="M35" s="21"/>
-      <c r="N35" s="21"/>
-      <c r="O35" s="21"/>
-      <c r="P35" s="21"/>
-      <c r="Q35" s="21"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="16"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="16"/>
+      <c r="Q35" s="16"/>
       <c r="R35" s="3"/>
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
@@ -3454,36 +3970,50 @@
       <c r="W35" s="3"/>
       <c r="X35" s="3"/>
       <c r="Y35" s="3"/>
-      <c r="Z35" s="3"/>
-    </row>
-    <row r="36" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z35" s="9">
+        <v>33</v>
+      </c>
+      <c r="AA35" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB35" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC35" s="9"/>
+      <c r="AD35" s="9"/>
+      <c r="AE35" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="AF35" s="9"/>
+    </row>
+    <row r="36" s="1" customFormat="1" ht="30" customHeight="1" spans="1:32">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="9">
+      <c r="F36" s="8">
         <v>3</v>
       </c>
-      <c r="G36" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="K36" s="10" t="s">
-        <v>165</v>
+      <c r="G36" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>215</v>
       </c>
       <c r="L36" s="3"/>
-      <c r="M36" s="21"/>
-      <c r="N36" s="21"/>
-      <c r="O36" s="21"/>
-      <c r="P36" s="21"/>
-      <c r="Q36" s="21"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="16"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="16"/>
+      <c r="Q36" s="16"/>
       <c r="R36" s="3"/>
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
@@ -3492,26 +4022,34 @@
       <c r="W36" s="3"/>
       <c r="X36" s="3"/>
       <c r="Y36" s="3"/>
-      <c r="Z36" s="3"/>
-    </row>
-    <row r="37" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z36" s="8">
+        <v>34</v>
+      </c>
+      <c r="AA36" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="AB36" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC36" s="9"/>
+      <c r="AD36" s="9"/>
+      <c r="AE36" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="AF36" s="9"/>
+    </row>
+    <row r="37" s="1" customFormat="1" ht="27" customHeight="1" spans="1:32">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
       <c r="L37" s="3"/>
-      <c r="M37" s="21"/>
-      <c r="N37" s="21"/>
-      <c r="O37" s="21"/>
-      <c r="P37" s="21"/>
-      <c r="Q37" s="21"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="16"/>
+      <c r="Q37" s="16"/>
       <c r="R37" s="3"/>
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
@@ -3520,20 +4058,28 @@
       <c r="W37" s="3"/>
       <c r="X37" s="3"/>
       <c r="Y37" s="3"/>
-      <c r="Z37" s="3"/>
-    </row>
-    <row r="38" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z37" s="8">
+        <v>35</v>
+      </c>
+      <c r="AA37" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="AB37" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC37" s="9"/>
+      <c r="AD37" s="9"/>
+      <c r="AE37" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="AF37" s="9"/>
+    </row>
+    <row r="38" s="1" customFormat="1" ht="24" customHeight="1" spans="1:32">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
@@ -3548,20 +4094,28 @@
       <c r="W38" s="3"/>
       <c r="X38" s="3"/>
       <c r="Y38" s="3"/>
-      <c r="Z38" s="3"/>
-    </row>
-    <row r="39" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z38" s="8">
+        <v>36</v>
+      </c>
+      <c r="AA38" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="AB38" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC38" s="9"/>
+      <c r="AD38" s="9"/>
+      <c r="AE38" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="AF38" s="9"/>
+    </row>
+    <row r="39" s="1" customFormat="1" ht="51" spans="1:32">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
@@ -3576,20 +4130,30 @@
       <c r="W39" s="3"/>
       <c r="X39" s="3"/>
       <c r="Y39" s="3"/>
-      <c r="Z39" s="3"/>
-    </row>
-    <row r="40" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z39" s="9">
+        <v>37</v>
+      </c>
+      <c r="AA39" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="AB39" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="AC39" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD39" s="9"/>
+      <c r="AE39" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="AF39" s="9"/>
+    </row>
+    <row r="40" s="1" customFormat="1" ht="38.25" spans="1:32">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
@@ -3604,20 +4168,32 @@
       <c r="W40" s="3"/>
       <c r="X40" s="3"/>
       <c r="Y40" s="3"/>
-      <c r="Z40" s="3"/>
-    </row>
-    <row r="41" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z40" s="9">
+        <v>38</v>
+      </c>
+      <c r="AA40" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="AB40" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="AC40" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD40" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="AE40" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF40" s="9"/>
+    </row>
+    <row r="41" s="1" customFormat="1" ht="63.75" spans="1:32">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
@@ -3632,20 +4208,30 @@
       <c r="W41" s="3"/>
       <c r="X41" s="3"/>
       <c r="Y41" s="3"/>
-      <c r="Z41" s="3"/>
-    </row>
-    <row r="42" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z41" s="9">
+        <v>39</v>
+      </c>
+      <c r="AA41" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="AB41" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="AC41" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD41" s="9"/>
+      <c r="AE41" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="AF41" s="9"/>
+    </row>
+    <row r="42" s="1" customFormat="1" ht="38.25" spans="1:32">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
@@ -3660,20 +4246,32 @@
       <c r="W42" s="3"/>
       <c r="X42" s="3"/>
       <c r="Y42" s="3"/>
-      <c r="Z42" s="3"/>
-    </row>
-    <row r="43" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z42" s="9">
+        <v>40</v>
+      </c>
+      <c r="AA42" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="AB42" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="AC42" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD42" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="AE42" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="AF42" s="9"/>
+    </row>
+    <row r="43" s="1" customFormat="1" ht="63.75" spans="1:32">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
@@ -3688,20 +4286,30 @@
       <c r="W43" s="3"/>
       <c r="X43" s="3"/>
       <c r="Y43" s="3"/>
-      <c r="Z43" s="3"/>
-    </row>
-    <row r="44" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z43" s="8">
+        <v>41</v>
+      </c>
+      <c r="AA43" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="AB43" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="AC43" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD43" s="9"/>
+      <c r="AE43" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="AF43" s="9"/>
+    </row>
+    <row r="44" s="1" customFormat="1" ht="51" spans="1:32">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
@@ -3716,20 +4324,32 @@
       <c r="W44" s="3"/>
       <c r="X44" s="3"/>
       <c r="Y44" s="3"/>
-      <c r="Z44" s="3"/>
-    </row>
-    <row r="45" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z44" s="8">
+        <v>42</v>
+      </c>
+      <c r="AA44" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="AB44" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="AC44" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD44" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="AE44" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="AF44" s="9"/>
+    </row>
+    <row r="45" s="1" customFormat="1" ht="51" spans="1:32">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
@@ -3744,20 +4364,30 @@
       <c r="W45" s="3"/>
       <c r="X45" s="3"/>
       <c r="Y45" s="3"/>
-      <c r="Z45" s="3"/>
-    </row>
-    <row r="46" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z45" s="8">
+        <v>43</v>
+      </c>
+      <c r="AA45" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="AB45" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="AC45" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD45" s="9"/>
+      <c r="AE45" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="AF45" s="9"/>
+    </row>
+    <row r="46" s="1" customFormat="1" ht="38.25" spans="1:32">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
@@ -3772,20 +4402,32 @@
       <c r="W46" s="3"/>
       <c r="X46" s="3"/>
       <c r="Y46" s="3"/>
-      <c r="Z46" s="3"/>
-    </row>
-    <row r="47" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z46" s="8">
+        <v>44</v>
+      </c>
+      <c r="AA46" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="AB46" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="AC46" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD46" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="AE46" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF46" s="21"/>
+    </row>
+    <row r="47" s="1" customFormat="1" ht="27" customHeight="1" spans="1:32">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
       <c r="N47" s="3"/>
@@ -3800,20 +4442,28 @@
       <c r="W47" s="3"/>
       <c r="X47" s="3"/>
       <c r="Y47" s="3"/>
-      <c r="Z47" s="3"/>
-    </row>
-    <row r="48" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z47" s="8">
+        <v>45</v>
+      </c>
+      <c r="AA47" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="AB47" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC47" s="9"/>
+      <c r="AD47" s="9"/>
+      <c r="AE47" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="AF47" s="9"/>
+    </row>
+    <row r="48" s="1" customFormat="1" ht="27" customHeight="1" spans="1:32">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
       <c r="N48" s="3"/>
@@ -3828,20 +4478,28 @@
       <c r="W48" s="3"/>
       <c r="X48" s="3"/>
       <c r="Y48" s="3"/>
-      <c r="Z48" s="3"/>
-    </row>
-    <row r="49" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+      <c r="Z48" s="8">
+        <v>46</v>
+      </c>
+      <c r="AA48" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="AB48" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="AC48" s="9"/>
+      <c r="AD48" s="9"/>
+      <c r="AE48" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="AF48" s="9"/>
+    </row>
+    <row r="49" s="1" customFormat="1" ht="27" customHeight="1" spans="1:25">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
@@ -3856,20 +4514,13 @@
       <c r="W49" s="3"/>
       <c r="X49" s="3"/>
       <c r="Y49" s="3"/>
-      <c r="Z49" s="3"/>
-    </row>
-    <row r="50" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+    </row>
+    <row r="50" s="1" customFormat="1" ht="27" customHeight="1" spans="1:25">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
@@ -3884,20 +4535,13 @@
       <c r="W50" s="3"/>
       <c r="X50" s="3"/>
       <c r="Y50" s="3"/>
-      <c r="Z50" s="3"/>
-    </row>
-    <row r="51" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+    </row>
+    <row r="51" s="1" customFormat="1" ht="27" customHeight="1" spans="1:25">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
@@ -3912,20 +4556,13 @@
       <c r="W51" s="3"/>
       <c r="X51" s="3"/>
       <c r="Y51" s="3"/>
-      <c r="Z51" s="3"/>
-    </row>
-    <row r="52" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+    </row>
+    <row r="52" s="1" customFormat="1" ht="27" customHeight="1" spans="1:25">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
       <c r="N52" s="3"/>
@@ -3940,9 +4577,8 @@
       <c r="W52" s="3"/>
       <c r="X52" s="3"/>
       <c r="Y52" s="3"/>
-      <c r="Z52" s="3"/>
-    </row>
-    <row r="53" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+    </row>
+    <row r="53" s="1" customFormat="1" ht="27" customHeight="1" spans="1:25">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -3968,9 +4604,8 @@
       <c r="W53" s="3"/>
       <c r="X53" s="3"/>
       <c r="Y53" s="3"/>
-      <c r="Z53" s="3"/>
-    </row>
-    <row r="54" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+    </row>
+    <row r="54" s="1" customFormat="1" ht="27" customHeight="1" spans="1:25">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -3996,9 +4631,8 @@
       <c r="W54" s="3"/>
       <c r="X54" s="3"/>
       <c r="Y54" s="3"/>
-      <c r="Z54" s="3"/>
-    </row>
-    <row r="55" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+    </row>
+    <row r="55" s="1" customFormat="1" ht="27" customHeight="1" spans="1:25">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -4024,9 +4658,8 @@
       <c r="W55" s="3"/>
       <c r="X55" s="3"/>
       <c r="Y55" s="3"/>
-      <c r="Z55" s="3"/>
-    </row>
-    <row r="56" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
+    </row>
+    <row r="56" s="1" customFormat="1" ht="27" customHeight="1" spans="1:25">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -4052,7 +4685,6 @@
       <c r="W56" s="3"/>
       <c r="X56" s="3"/>
       <c r="Y56" s="3"/>
-      <c r="Z56" s="3"/>
     </row>
     <row r="57" s="1" customFormat="1" ht="27" customHeight="1" spans="1:26">
       <c r="A57" s="3"/>

</xml_diff>